<commit_message>
Running CIs and CRIs
</commit_message>
<xml_diff>
--- a/Sim_DataFrame_Plan.xlsx
+++ b/Sim_DataFrame_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conorlacey/Documents/Grad School/Research/Thesis/Thesis R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D3DD57-FEA6-6C45-B402-485BE4B5A8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267CB4FC-AE38-C540-BE1A-8C5373F95D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="1880" windowWidth="23820" windowHeight="17500" xr2:uid="{2CE5E951-8CB5-3C4B-AF22-C52294E8CEFF}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="23820" windowHeight="17500" xr2:uid="{2CE5E951-8CB5-3C4B-AF22-C52294E8CEFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>Each cell will be the mean estimate after 500 replications.</t>
   </si>
@@ -126,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -255,11 +255,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -286,16 +310,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DB3B1C-C16F-EB40-8F32-8665E0986627}">
-  <dimension ref="A1:S70"/>
+  <dimension ref="A1:Y68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="90" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="K67" sqref="K67"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="64" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="X61" sqref="X61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1539,10 +1576,10 @@
       </c>
       <c r="M32" s="16"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="M33" s="16"/>
     </row>
-    <row r="34" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>1</v>
       </c>
@@ -1559,7 +1596,7 @@
       <c r="L34" s="19"/>
       <c r="M34" s="16"/>
     </row>
-    <row r="35" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="20" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>0.25</v>
       </c>
@@ -1598,7 +1635,7 @@
       </c>
       <c r="M35" s="16"/>
     </row>
-    <row r="36" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>250</v>
       </c>
@@ -1637,7 +1674,7 @@
       </c>
       <c r="M36" s="16"/>
     </row>
-    <row r="37" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>500</v>
       </c>
@@ -1676,7 +1713,7 @@
       </c>
       <c r="M37" s="16"/>
     </row>
-    <row r="38" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>1000</v>
       </c>
@@ -1715,7 +1752,7 @@
       </c>
       <c r="M38" s="16"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1730,443 +1767,1030 @@
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-    </row>
-    <row r="43" spans="1:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="20"/>
-    </row>
-    <row r="44" spans="1:13" ht="20" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="20"/>
-    </row>
-    <row r="45" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="24"/>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="15"/>
+      <c r="V42" s="15"/>
+    </row>
+    <row r="43" spans="1:25" ht="21" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
+        <v>0</v>
+      </c>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
+      <c r="T43" s="18"/>
+      <c r="U43" s="19"/>
+      <c r="V43" s="15"/>
+      <c r="X43" s="15"/>
+      <c r="Y43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="20" x14ac:dyDescent="0.25">
+      <c r="A44" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="B44" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="G44" s="29"/>
+      <c r="H44" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="I44" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="N44" s="29"/>
+      <c r="O44" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="P44" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="Q44" s="27"/>
+      <c r="R44" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="S44" s="27"/>
+      <c r="T44" s="27">
+        <v>0.9</v>
+      </c>
+      <c r="U44" s="28"/>
+      <c r="V44" s="15"/>
+    </row>
+    <row r="45" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="A45" s="30">
+        <v>250</v>
+      </c>
+      <c r="B45" s="31">
+        <v>1</v>
+      </c>
+      <c r="C45" s="23"/>
+      <c r="D45" s="31">
+        <v>4</v>
+      </c>
+      <c r="E45" s="23"/>
+      <c r="F45" s="22">
+        <v>7</v>
+      </c>
       <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="20"/>
-    </row>
-    <row r="46" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="24"/>
+      <c r="H45" s="30">
+        <v>250</v>
+      </c>
+      <c r="I45" s="31">
+        <v>10</v>
+      </c>
+      <c r="J45" s="23"/>
+      <c r="K45" s="31">
+        <v>13</v>
+      </c>
+      <c r="L45" s="23"/>
+      <c r="M45" s="22">
+        <v>16</v>
+      </c>
+      <c r="N45" s="24"/>
+      <c r="O45" s="30">
+        <v>250</v>
+      </c>
+      <c r="P45" s="34">
+        <v>19</v>
+      </c>
+      <c r="Q45" s="23"/>
+      <c r="R45" s="31">
+        <v>22</v>
+      </c>
+      <c r="S45" s="23"/>
+      <c r="T45" s="22">
+        <v>25</v>
+      </c>
+      <c r="U45" s="24"/>
+      <c r="V45" s="15"/>
+    </row>
+    <row r="46" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="A46" s="30">
+        <v>500</v>
+      </c>
+      <c r="B46" s="32">
+        <v>2</v>
+      </c>
       <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="24"/>
+      <c r="D46" s="32">
+        <v>5</v>
+      </c>
+      <c r="E46" s="24"/>
+      <c r="F46" s="22">
+        <v>8</v>
+      </c>
       <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="22"/>
+      <c r="H46" s="30">
+        <v>500</v>
+      </c>
+      <c r="I46" s="32">
+        <v>11</v>
+      </c>
       <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
+      <c r="K46" s="32">
+        <v>14</v>
+      </c>
       <c r="L46" s="24"/>
-      <c r="M46" s="20"/>
-    </row>
-    <row r="47" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="27"/>
-      <c r="M47" s="20"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="20"/>
-      <c r="L48" s="20"/>
-      <c r="M48" s="20"/>
-    </row>
-    <row r="49" spans="1:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="20"/>
-    </row>
-    <row r="50" spans="1:13" ht="20" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="20"/>
-    </row>
-    <row r="51" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="24"/>
+      <c r="M46" s="22">
+        <v>17</v>
+      </c>
+      <c r="N46" s="24"/>
+      <c r="O46" s="30">
+        <v>500</v>
+      </c>
+      <c r="P46" s="22">
+        <v>20</v>
+      </c>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="32">
+        <v>23</v>
+      </c>
+      <c r="S46" s="24"/>
+      <c r="T46" s="22">
+        <v>26</v>
+      </c>
+      <c r="U46" s="24"/>
+      <c r="V46" s="15"/>
+    </row>
+    <row r="47" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="A47" s="30">
+        <v>1000</v>
+      </c>
+      <c r="B47" s="33">
+        <v>3</v>
+      </c>
+      <c r="C47" s="25"/>
+      <c r="D47" s="33">
+        <v>6</v>
+      </c>
+      <c r="E47" s="25"/>
+      <c r="F47" s="6">
+        <v>9</v>
+      </c>
+      <c r="G47" s="25"/>
+      <c r="H47" s="30">
+        <v>1000</v>
+      </c>
+      <c r="I47" s="33">
+        <v>12</v>
+      </c>
+      <c r="J47" s="25"/>
+      <c r="K47" s="33">
+        <v>15</v>
+      </c>
+      <c r="L47" s="25"/>
+      <c r="M47" s="6">
+        <v>18</v>
+      </c>
+      <c r="N47" s="25"/>
+      <c r="O47" s="30">
+        <v>1000</v>
+      </c>
+      <c r="P47" s="6">
+        <v>21</v>
+      </c>
+      <c r="Q47" s="25"/>
+      <c r="R47" s="33">
+        <v>24</v>
+      </c>
+      <c r="S47" s="25"/>
+      <c r="T47" s="6">
+        <v>27</v>
+      </c>
+      <c r="U47" s="25"/>
+      <c r="V47" s="15"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="V48" s="15"/>
+    </row>
+    <row r="49" spans="1:25" ht="21" x14ac:dyDescent="0.25">
+      <c r="A49" s="17">
+        <v>1</v>
+      </c>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
+      <c r="Q49" s="18"/>
+      <c r="R49" s="18"/>
+      <c r="S49" s="18"/>
+      <c r="T49" s="18"/>
+      <c r="U49" s="19"/>
+      <c r="V49" s="15"/>
+    </row>
+    <row r="50" spans="1:25" ht="20" x14ac:dyDescent="0.25">
+      <c r="A50" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="B50" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E50" s="29"/>
+      <c r="F50" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G50" s="28"/>
+      <c r="H50" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="I50" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="N50" s="29"/>
+      <c r="O50" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="P50" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="S50" s="29"/>
+      <c r="T50" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="U50" s="29"/>
+      <c r="V50" s="15"/>
+    </row>
+    <row r="51" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="A51" s="30">
+        <v>250</v>
+      </c>
+      <c r="B51" s="31">
+        <v>28</v>
+      </c>
+      <c r="C51" s="23"/>
+      <c r="D51" s="31">
+        <v>31</v>
+      </c>
+      <c r="E51" s="23"/>
+      <c r="F51" s="22">
+        <v>34</v>
+      </c>
       <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="24"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="20"/>
-    </row>
-    <row r="52" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="24"/>
+      <c r="H51" s="30">
+        <v>250</v>
+      </c>
+      <c r="I51" s="31">
+        <v>37</v>
+      </c>
+      <c r="J51" s="23"/>
+      <c r="K51" s="31">
+        <v>40</v>
+      </c>
+      <c r="L51" s="23"/>
+      <c r="M51" s="22">
+        <v>43</v>
+      </c>
+      <c r="N51" s="24"/>
+      <c r="O51" s="30">
+        <v>250</v>
+      </c>
+      <c r="P51" s="34">
+        <v>46</v>
+      </c>
+      <c r="Q51" s="23"/>
+      <c r="R51" s="31">
+        <v>49</v>
+      </c>
+      <c r="S51" s="23"/>
+      <c r="T51" s="22">
+        <v>52</v>
+      </c>
+      <c r="U51" s="24"/>
+      <c r="V51" s="15"/>
+    </row>
+    <row r="52" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="A52" s="30">
+        <v>500</v>
+      </c>
+      <c r="B52" s="32">
+        <v>29</v>
+      </c>
       <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="24"/>
+      <c r="D52" s="32">
+        <v>32</v>
+      </c>
+      <c r="E52" s="24"/>
+      <c r="F52" s="22">
+        <v>35</v>
+      </c>
       <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="22"/>
+      <c r="H52" s="30">
+        <v>500</v>
+      </c>
+      <c r="I52" s="32">
+        <v>38</v>
+      </c>
       <c r="J52" s="24"/>
-      <c r="K52" s="24"/>
+      <c r="K52" s="32">
+        <v>41</v>
+      </c>
       <c r="L52" s="24"/>
-      <c r="M52" s="20"/>
-    </row>
-    <row r="53" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="22"/>
-      <c r="J53" s="24"/>
-      <c r="K53" s="24"/>
-      <c r="L53" s="24"/>
-      <c r="M53" s="20"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="20"/>
-      <c r="L54" s="20"/>
-      <c r="M54" s="20"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A55" s="20"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="20"/>
-      <c r="L55" s="20"/>
-      <c r="M55" s="20"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="20"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
-      <c r="K56" s="20"/>
-      <c r="L56" s="20"/>
-      <c r="M56" s="20"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="20"/>
-      <c r="J57" s="20"/>
-      <c r="K57" s="20"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="20"/>
-    </row>
-    <row r="58" spans="1:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="A58" s="25"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-      <c r="I58" s="25"/>
-      <c r="J58" s="25"/>
-      <c r="K58" s="25"/>
-      <c r="L58" s="25"/>
-      <c r="M58" s="20"/>
-    </row>
-    <row r="59" spans="1:13" ht="20" x14ac:dyDescent="0.25">
-      <c r="A59" s="21"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
+      <c r="M52" s="22">
+        <v>44</v>
+      </c>
+      <c r="N52" s="24"/>
+      <c r="O52" s="30">
+        <v>500</v>
+      </c>
+      <c r="P52" s="22">
+        <v>47</v>
+      </c>
+      <c r="Q52" s="24"/>
+      <c r="R52" s="32">
+        <v>50</v>
+      </c>
+      <c r="S52" s="24"/>
+      <c r="T52" s="22">
+        <v>53</v>
+      </c>
+      <c r="U52" s="24"/>
+      <c r="V52" s="15"/>
+    </row>
+    <row r="53" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="A53" s="30">
+        <v>1000</v>
+      </c>
+      <c r="B53" s="33">
+        <v>30</v>
+      </c>
+      <c r="C53" s="25"/>
+      <c r="D53" s="33">
+        <v>33</v>
+      </c>
+      <c r="E53" s="25"/>
+      <c r="F53" s="6">
+        <v>36</v>
+      </c>
+      <c r="G53" s="25"/>
+      <c r="H53" s="30">
+        <v>1000</v>
+      </c>
+      <c r="I53" s="33">
+        <v>39</v>
+      </c>
+      <c r="J53" s="25"/>
+      <c r="K53" s="33">
+        <v>42</v>
+      </c>
+      <c r="L53" s="25"/>
+      <c r="M53" s="6">
+        <v>45</v>
+      </c>
+      <c r="N53" s="25"/>
+      <c r="O53" s="30">
+        <v>1000</v>
+      </c>
+      <c r="P53" s="6">
+        <v>48</v>
+      </c>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="33">
+        <v>51</v>
+      </c>
+      <c r="S53" s="25"/>
+      <c r="T53" s="6">
+        <v>54</v>
+      </c>
+      <c r="U53" s="25"/>
+      <c r="V53" s="15"/>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="15"/>
+      <c r="T54" s="15"/>
+      <c r="U54" s="15"/>
+      <c r="V54" s="15"/>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="16"/>
+      <c r="T56" s="16"/>
+      <c r="U56" s="16"/>
+      <c r="V56" s="16"/>
+    </row>
+    <row r="57" spans="1:25" ht="21" x14ac:dyDescent="0.25">
+      <c r="A57" s="17">
+        <v>0</v>
+      </c>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
+      <c r="P57" s="18"/>
+      <c r="Q57" s="18"/>
+      <c r="R57" s="18"/>
+      <c r="S57" s="18"/>
+      <c r="T57" s="18"/>
+      <c r="U57" s="19"/>
+      <c r="V57" s="16"/>
+      <c r="X57" s="16"/>
+      <c r="Y57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" ht="20" x14ac:dyDescent="0.25">
+      <c r="A58" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="B58" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="G58" s="29"/>
+      <c r="H58" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="I58" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="J58" s="29"/>
+      <c r="K58" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="L58" s="29"/>
+      <c r="M58" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="N58" s="29"/>
+      <c r="O58" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="P58" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="Q58" s="27"/>
+      <c r="R58" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="S58" s="27"/>
+      <c r="T58" s="27">
+        <v>0.9</v>
+      </c>
+      <c r="U58" s="28"/>
+      <c r="V58" s="16"/>
+    </row>
+    <row r="59" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="A59" s="30">
+        <v>250</v>
+      </c>
+      <c r="B59" s="31">
+        <v>1</v>
+      </c>
+      <c r="C59" s="23"/>
+      <c r="D59" s="31">
+        <v>4</v>
+      </c>
       <c r="E59" s="23"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="23"/>
-      <c r="J59" s="22"/>
-      <c r="K59" s="22"/>
-      <c r="L59" s="22"/>
-      <c r="M59" s="20"/>
-    </row>
-    <row r="60" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="24"/>
+      <c r="F59" s="22">
+        <v>7</v>
+      </c>
+      <c r="G59" s="24"/>
+      <c r="H59" s="30">
+        <v>250</v>
+      </c>
+      <c r="I59" s="31">
+        <v>10</v>
+      </c>
+      <c r="J59" s="23"/>
+      <c r="K59" s="31">
+        <v>13</v>
+      </c>
+      <c r="L59" s="23"/>
+      <c r="M59" s="22">
+        <v>16</v>
+      </c>
+      <c r="N59" s="24"/>
+      <c r="O59" s="30">
+        <v>250</v>
+      </c>
+      <c r="P59" s="34">
+        <v>19</v>
+      </c>
+      <c r="Q59" s="23"/>
+      <c r="R59" s="31">
+        <v>22</v>
+      </c>
+      <c r="S59" s="23"/>
+      <c r="T59" s="22">
+        <v>25</v>
+      </c>
+      <c r="U59" s="24"/>
+      <c r="V59" s="16"/>
+    </row>
+    <row r="60" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="A60" s="30">
+        <v>500</v>
+      </c>
+      <c r="B60" s="32">
+        <v>2</v>
+      </c>
       <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="24"/>
+      <c r="D60" s="32">
+        <v>5</v>
+      </c>
+      <c r="E60" s="24"/>
+      <c r="F60" s="22">
+        <v>8</v>
+      </c>
       <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="22"/>
+      <c r="H60" s="30">
+        <v>500</v>
+      </c>
+      <c r="I60" s="32">
+        <v>11</v>
+      </c>
       <c r="J60" s="24"/>
-      <c r="K60" s="24"/>
+      <c r="K60" s="32">
+        <v>14</v>
+      </c>
       <c r="L60" s="24"/>
-      <c r="M60" s="20"/>
-    </row>
-    <row r="61" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="24"/>
-      <c r="G61" s="24"/>
-      <c r="H61" s="24"/>
-      <c r="I61" s="22"/>
-      <c r="J61" s="24"/>
-      <c r="K61" s="24"/>
-      <c r="L61" s="24"/>
-      <c r="M61" s="20"/>
-    </row>
-    <row r="62" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="22"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="24"/>
-      <c r="H62" s="24"/>
-      <c r="I62" s="22"/>
-      <c r="J62" s="24"/>
-      <c r="K62" s="24"/>
-      <c r="L62" s="24"/>
-      <c r="M62" s="20"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A63" s="20"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="20"/>
-      <c r="I63" s="20"/>
-      <c r="J63" s="20"/>
-      <c r="K63" s="20"/>
-      <c r="L63" s="20"/>
-      <c r="M63" s="20"/>
-    </row>
-    <row r="64" spans="1:13" ht="21" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
-      <c r="I64" s="25"/>
-      <c r="J64" s="25"/>
-      <c r="K64" s="25"/>
-      <c r="L64" s="25"/>
-      <c r="M64" s="20"/>
-    </row>
-    <row r="65" spans="1:13" ht="20" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="B65" s="22"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="22"/>
+      <c r="M60" s="22">
+        <v>17</v>
+      </c>
+      <c r="N60" s="24"/>
+      <c r="O60" s="30">
+        <v>500</v>
+      </c>
+      <c r="P60" s="22">
+        <v>20</v>
+      </c>
+      <c r="Q60" s="24"/>
+      <c r="R60" s="32">
+        <v>23</v>
+      </c>
+      <c r="S60" s="24"/>
+      <c r="T60" s="22">
+        <v>26</v>
+      </c>
+      <c r="U60" s="24"/>
+      <c r="V60" s="16"/>
+    </row>
+    <row r="61" spans="1:25" ht="19" x14ac:dyDescent="0.25">
+      <c r="A61" s="30">
+        <v>1000</v>
+      </c>
+      <c r="B61" s="33">
+        <v>3</v>
+      </c>
+      <c r="C61" s="25"/>
+      <c r="D61" s="33">
+        <v>6</v>
+      </c>
+      <c r="E61" s="25"/>
+      <c r="F61" s="6">
+        <v>9</v>
+      </c>
+      <c r="G61" s="25"/>
+      <c r="H61" s="30">
+        <v>1000</v>
+      </c>
+      <c r="I61" s="33">
+        <v>12</v>
+      </c>
+      <c r="J61" s="25"/>
+      <c r="K61" s="33">
+        <v>15</v>
+      </c>
+      <c r="L61" s="25"/>
+      <c r="M61" s="6">
+        <v>18</v>
+      </c>
+      <c r="N61" s="25"/>
+      <c r="O61" s="30">
+        <v>1000</v>
+      </c>
+      <c r="P61" s="6">
+        <v>21</v>
+      </c>
+      <c r="Q61" s="25"/>
+      <c r="R61" s="33">
+        <v>24</v>
+      </c>
+      <c r="S61" s="25"/>
+      <c r="T61" s="6">
+        <v>27</v>
+      </c>
+      <c r="U61" s="25"/>
+      <c r="V61" s="16"/>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="V62" s="16"/>
+    </row>
+    <row r="63" spans="1:25" ht="21" x14ac:dyDescent="0.25">
+      <c r="A63" s="17">
+        <v>1</v>
+      </c>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="18"/>
+      <c r="M63" s="18"/>
+      <c r="N63" s="18"/>
+      <c r="O63" s="18"/>
+      <c r="P63" s="18"/>
+      <c r="Q63" s="18"/>
+      <c r="R63" s="18"/>
+      <c r="S63" s="18"/>
+      <c r="T63" s="18"/>
+      <c r="U63" s="19"/>
+      <c r="V63" s="16"/>
+    </row>
+    <row r="64" spans="1:25" ht="20" x14ac:dyDescent="0.25">
+      <c r="A64" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="B64" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E64" s="29"/>
+      <c r="F64" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="G64" s="28"/>
+      <c r="H64" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="I64" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="J64" s="29"/>
+      <c r="K64" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="L64" s="29"/>
+      <c r="M64" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="N64" s="29"/>
+      <c r="O64" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="P64" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="Q64" s="29"/>
+      <c r="R64" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="S64" s="29"/>
+      <c r="T64" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="U64" s="29"/>
+      <c r="V64" s="16"/>
+    </row>
+    <row r="65" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A65" s="30">
+        <v>250</v>
+      </c>
+      <c r="B65" s="31">
+        <v>28</v>
+      </c>
+      <c r="C65" s="23"/>
+      <c r="D65" s="31">
+        <v>31</v>
+      </c>
       <c r="E65" s="23"/>
-      <c r="F65" s="22"/>
-      <c r="G65" s="22"/>
-      <c r="H65" s="22"/>
-      <c r="I65" s="23"/>
-      <c r="J65" s="22"/>
-      <c r="K65" s="22"/>
-      <c r="L65" s="22"/>
-      <c r="M65" s="20"/>
-    </row>
-    <row r="66" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A66" s="22"/>
-      <c r="B66" s="24"/>
+      <c r="F65" s="22">
+        <v>34</v>
+      </c>
+      <c r="G65" s="24"/>
+      <c r="H65" s="30">
+        <v>250</v>
+      </c>
+      <c r="I65" s="31">
+        <v>37</v>
+      </c>
+      <c r="J65" s="23"/>
+      <c r="K65" s="31">
+        <v>40</v>
+      </c>
+      <c r="L65" s="23"/>
+      <c r="M65" s="22">
+        <v>43</v>
+      </c>
+      <c r="N65" s="24"/>
+      <c r="O65" s="30">
+        <v>250</v>
+      </c>
+      <c r="P65" s="34">
+        <v>46</v>
+      </c>
+      <c r="Q65" s="23"/>
+      <c r="R65" s="31">
+        <v>49</v>
+      </c>
+      <c r="S65" s="23"/>
+      <c r="T65" s="22">
+        <v>52</v>
+      </c>
+      <c r="U65" s="24"/>
+      <c r="V65" s="16"/>
+    </row>
+    <row r="66" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A66" s="30">
+        <v>500</v>
+      </c>
+      <c r="B66" s="32">
+        <v>29</v>
+      </c>
       <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="22"/>
-      <c r="F66" s="24"/>
+      <c r="D66" s="32">
+        <v>32</v>
+      </c>
+      <c r="E66" s="24"/>
+      <c r="F66" s="22">
+        <v>35</v>
+      </c>
       <c r="G66" s="24"/>
-      <c r="H66" s="24"/>
-      <c r="I66" s="22"/>
+      <c r="H66" s="30">
+        <v>500</v>
+      </c>
+      <c r="I66" s="32">
+        <v>38</v>
+      </c>
       <c r="J66" s="24"/>
-      <c r="K66" s="24"/>
+      <c r="K66" s="32">
+        <v>41</v>
+      </c>
       <c r="L66" s="24"/>
-      <c r="M66" s="20"/>
-    </row>
-    <row r="67" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A67" s="22"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="24"/>
-      <c r="H67" s="24"/>
-      <c r="I67" s="22"/>
-      <c r="J67" s="24"/>
-      <c r="K67" s="24"/>
-      <c r="L67" s="24"/>
-      <c r="M67" s="20"/>
-    </row>
-    <row r="68" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A68" s="22"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="24"/>
-      <c r="H68" s="24"/>
-      <c r="I68" s="22"/>
-      <c r="J68" s="24"/>
-      <c r="K68" s="24"/>
-      <c r="L68" s="24"/>
-      <c r="M68" s="20"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="20"/>
-      <c r="H69" s="20"/>
-      <c r="I69" s="20"/>
-      <c r="J69" s="20"/>
-      <c r="K69" s="20"/>
-      <c r="L69" s="20"/>
-      <c r="M69" s="20"/>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A70" s="20"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="20"/>
-      <c r="H70" s="20"/>
-      <c r="I70" s="20"/>
-      <c r="J70" s="20"/>
-      <c r="K70" s="20"/>
-      <c r="L70" s="20"/>
-      <c r="M70" s="20"/>
+      <c r="M66" s="22">
+        <v>44</v>
+      </c>
+      <c r="N66" s="24"/>
+      <c r="O66" s="30">
+        <v>500</v>
+      </c>
+      <c r="P66" s="22">
+        <v>47</v>
+      </c>
+      <c r="Q66" s="24"/>
+      <c r="R66" s="32">
+        <v>50</v>
+      </c>
+      <c r="S66" s="24"/>
+      <c r="T66" s="22">
+        <v>53</v>
+      </c>
+      <c r="U66" s="24"/>
+      <c r="V66" s="16"/>
+    </row>
+    <row r="67" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A67" s="30">
+        <v>1000</v>
+      </c>
+      <c r="B67" s="33">
+        <v>30</v>
+      </c>
+      <c r="C67" s="25"/>
+      <c r="D67" s="33">
+        <v>33</v>
+      </c>
+      <c r="E67" s="25"/>
+      <c r="F67" s="6">
+        <v>36</v>
+      </c>
+      <c r="G67" s="25"/>
+      <c r="H67" s="30">
+        <v>1000</v>
+      </c>
+      <c r="I67" s="33">
+        <v>39</v>
+      </c>
+      <c r="J67" s="25"/>
+      <c r="K67" s="33">
+        <v>42</v>
+      </c>
+      <c r="L67" s="25"/>
+      <c r="M67" s="6">
+        <v>45</v>
+      </c>
+      <c r="N67" s="25"/>
+      <c r="O67" s="30">
+        <v>1000</v>
+      </c>
+      <c r="P67" s="6">
+        <v>48</v>
+      </c>
+      <c r="Q67" s="25"/>
+      <c r="R67" s="33">
+        <v>51</v>
+      </c>
+      <c r="S67" s="25"/>
+      <c r="T67" s="6">
+        <v>54</v>
+      </c>
+      <c r="U67" s="25"/>
+      <c r="V67" s="16"/>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A68" s="16"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="16"/>
+      <c r="J68" s="16"/>
+      <c r="K68" s="16"/>
+      <c r="L68" s="16"/>
+      <c r="M68" s="16"/>
+      <c r="N68" s="16"/>
+      <c r="O68" s="16"/>
+      <c r="P68" s="16"/>
+      <c r="Q68" s="16"/>
+      <c r="R68" s="16"/>
+      <c r="S68" s="16"/>
+      <c r="T68" s="16"/>
+      <c r="U68" s="16"/>
+      <c r="V68" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="46">
+    <mergeCell ref="A63:U63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="P64:Q64"/>
+    <mergeCell ref="R64:S64"/>
+    <mergeCell ref="T64:U64"/>
+    <mergeCell ref="A43:U43"/>
+    <mergeCell ref="A57:U57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="R58:S58"/>
+    <mergeCell ref="T58:U58"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="R44:S44"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="P50:Q50"/>
+    <mergeCell ref="R50:S50"/>
+    <mergeCell ref="T50:U50"/>
+    <mergeCell ref="A49:U49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:L44"/>
     <mergeCell ref="A28:L28"/>
     <mergeCell ref="A34:L34"/>
     <mergeCell ref="A1:L1"/>

</xml_diff>

<commit_message>
Proportion of No Effect Analysis
</commit_message>
<xml_diff>
--- a/Sim_DataFrame_Plan.xlsx
+++ b/Sim_DataFrame_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conorlacey/Documents/Grad School/Research/Thesis/Thesis R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777D60F4-0F00-0947-B28D-EC3389E3402C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D6827D-3346-E344-A7D9-B4B5F25A7D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2CE5E951-8CB5-3C4B-AF22-C52294E8CEFF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Each cell will be the mean estimate after 500 replications.</t>
   </si>
@@ -47,17 +47,32 @@
     <t>dMACS_Shrunk</t>
   </si>
   <si>
-    <t>dMACS_Post</t>
+    <t>dMACS_post</t>
   </si>
   <si>
-    <t>dMACS_post</t>
+    <t>dMACS CI</t>
+  </si>
+  <si>
+    <t>dMACS_Post CRI</t>
+  </si>
+  <si>
+    <t>dMACS_Shrunk CRI</t>
+  </si>
+  <si>
+    <t>dMACS Props No Effect</t>
+  </si>
+  <si>
+    <t>dMACS_Post Props No Effect</t>
+  </si>
+  <si>
+    <t>dMACS_Shrunk Props No Effect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,8 +126,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +190,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -291,11 +356,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -338,6 +416,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DB3B1C-C16F-EB40-8F32-8665E0986627}">
-  <dimension ref="A1:Y98"/>
+  <dimension ref="A1:Y140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="U98" sqref="U98"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="75" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="M139" sqref="M139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1422,7 +1519,7 @@
       <c r="M28" s="30"/>
       <c r="O28" s="30"/>
       <c r="P28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="20" x14ac:dyDescent="0.25">
@@ -2206,7 +2303,7 @@
       <c r="V57" s="13"/>
       <c r="X57" s="13"/>
       <c r="Y57" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:25" ht="20" x14ac:dyDescent="0.25">
@@ -2805,7 +2902,7 @@
       <c r="V72" s="30"/>
       <c r="X72" s="30"/>
       <c r="Y72" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:25" ht="20" x14ac:dyDescent="0.25">
@@ -3404,7 +3501,7 @@
       <c r="V87" s="14"/>
       <c r="X87" s="14"/>
       <c r="Y87" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:25" ht="20" x14ac:dyDescent="0.25">
@@ -3952,8 +4049,1190 @@
       <c r="U98" s="14"/>
       <c r="V98" s="14"/>
     </row>
+    <row r="100" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A100" s="13"/>
+      <c r="B100" s="13"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="13"/>
+      <c r="K100" s="13"/>
+      <c r="L100" s="13"/>
+      <c r="M100" s="13"/>
+    </row>
+    <row r="101" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+      <c r="A101" s="25">
+        <v>0</v>
+      </c>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="26"/>
+      <c r="F101" s="26"/>
+      <c r="G101" s="26"/>
+      <c r="H101" s="26"/>
+      <c r="I101" s="26"/>
+      <c r="J101" s="26"/>
+      <c r="K101" s="26"/>
+      <c r="L101" s="27"/>
+      <c r="M101" s="13"/>
+      <c r="O101" s="13"/>
+      <c r="P101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:22" ht="20" x14ac:dyDescent="0.25">
+      <c r="A102" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="B102" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="C102" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D102" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="E102" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F102" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="G102" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="H102" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="I102" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J102" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="K102" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="L102" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="M102" s="13"/>
+    </row>
+    <row r="103" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A103" s="20">
+        <v>250</v>
+      </c>
+      <c r="B103" s="4">
+        <v>100</v>
+      </c>
+      <c r="C103" s="4">
+        <v>0</v>
+      </c>
+      <c r="D103" s="5">
+        <v>0</v>
+      </c>
+      <c r="E103" s="20">
+        <v>250</v>
+      </c>
+      <c r="F103" s="4">
+        <v>100</v>
+      </c>
+      <c r="G103" s="4">
+        <v>0</v>
+      </c>
+      <c r="H103" s="5">
+        <v>0</v>
+      </c>
+      <c r="I103" s="20">
+        <v>250</v>
+      </c>
+      <c r="J103" s="4">
+        <v>100</v>
+      </c>
+      <c r="K103" s="4">
+        <v>0</v>
+      </c>
+      <c r="L103" s="5">
+        <v>0</v>
+      </c>
+      <c r="M103" s="13"/>
+    </row>
+    <row r="104" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A104" s="20">
+        <v>500</v>
+      </c>
+      <c r="B104" s="4">
+        <v>0</v>
+      </c>
+      <c r="C104" s="4">
+        <v>0</v>
+      </c>
+      <c r="D104" s="5">
+        <v>0</v>
+      </c>
+      <c r="E104" s="20">
+        <v>500</v>
+      </c>
+      <c r="F104" s="4">
+        <v>0</v>
+      </c>
+      <c r="G104" s="4">
+        <v>0</v>
+      </c>
+      <c r="H104" s="5">
+        <v>0</v>
+      </c>
+      <c r="I104" s="20">
+        <v>500</v>
+      </c>
+      <c r="J104" s="4">
+        <v>0</v>
+      </c>
+      <c r="K104" s="4">
+        <v>0</v>
+      </c>
+      <c r="L104" s="5">
+        <v>0</v>
+      </c>
+      <c r="M104" s="13"/>
+    </row>
+    <row r="105" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A105" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B105" s="6">
+        <v>0</v>
+      </c>
+      <c r="C105" s="6">
+        <v>0</v>
+      </c>
+      <c r="D105" s="7">
+        <v>0</v>
+      </c>
+      <c r="E105" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F105" s="6">
+        <v>0</v>
+      </c>
+      <c r="G105" s="6">
+        <v>0</v>
+      </c>
+      <c r="H105" s="7">
+        <v>0</v>
+      </c>
+      <c r="I105" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J105" s="6">
+        <v>0</v>
+      </c>
+      <c r="K105" s="6">
+        <v>0</v>
+      </c>
+      <c r="L105" s="7">
+        <v>0</v>
+      </c>
+      <c r="M105" s="13"/>
+    </row>
+    <row r="106" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M106" s="13"/>
+    </row>
+    <row r="107" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+      <c r="A107" s="25">
+        <v>1</v>
+      </c>
+      <c r="B107" s="26"/>
+      <c r="C107" s="26"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="26"/>
+      <c r="F107" s="26"/>
+      <c r="G107" s="26"/>
+      <c r="H107" s="26"/>
+      <c r="I107" s="26"/>
+      <c r="J107" s="26"/>
+      <c r="K107" s="26"/>
+      <c r="L107" s="27"/>
+      <c r="M107" s="13"/>
+    </row>
+    <row r="108" spans="1:22" ht="20" x14ac:dyDescent="0.25">
+      <c r="A108" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="B108" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="C108" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D108" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="E108" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F108" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="G108" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="H108" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="I108" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J108" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="K108" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="L108" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="M108" s="13"/>
+    </row>
+    <row r="109" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A109" s="20">
+        <v>250</v>
+      </c>
+      <c r="B109" s="4">
+        <v>100</v>
+      </c>
+      <c r="C109" s="4">
+        <v>0</v>
+      </c>
+      <c r="D109" s="5">
+        <v>0</v>
+      </c>
+      <c r="E109" s="20">
+        <v>250</v>
+      </c>
+      <c r="F109" s="4">
+        <v>100</v>
+      </c>
+      <c r="G109" s="4">
+        <v>0</v>
+      </c>
+      <c r="H109" s="5">
+        <v>0</v>
+      </c>
+      <c r="I109" s="20">
+        <v>250</v>
+      </c>
+      <c r="J109" s="4">
+        <v>100</v>
+      </c>
+      <c r="K109" s="4">
+        <v>0</v>
+      </c>
+      <c r="L109" s="5">
+        <v>0</v>
+      </c>
+      <c r="M109" s="13"/>
+    </row>
+    <row r="110" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A110" s="20">
+        <v>500</v>
+      </c>
+      <c r="B110" s="4">
+        <v>0</v>
+      </c>
+      <c r="C110" s="4">
+        <v>0</v>
+      </c>
+      <c r="D110" s="5">
+        <v>0</v>
+      </c>
+      <c r="E110" s="20">
+        <v>500</v>
+      </c>
+      <c r="F110" s="4">
+        <v>0</v>
+      </c>
+      <c r="G110" s="4">
+        <v>0</v>
+      </c>
+      <c r="H110" s="5">
+        <v>0</v>
+      </c>
+      <c r="I110" s="20">
+        <v>500</v>
+      </c>
+      <c r="J110" s="4">
+        <v>0</v>
+      </c>
+      <c r="K110" s="4">
+        <v>0</v>
+      </c>
+      <c r="L110" s="5">
+        <v>0</v>
+      </c>
+      <c r="M110" s="13"/>
+    </row>
+    <row r="111" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A111" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B111" s="6">
+        <v>0</v>
+      </c>
+      <c r="C111" s="6">
+        <v>0</v>
+      </c>
+      <c r="D111" s="7">
+        <v>0</v>
+      </c>
+      <c r="E111" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F111" s="6">
+        <v>0</v>
+      </c>
+      <c r="G111" s="6">
+        <v>0</v>
+      </c>
+      <c r="H111" s="7">
+        <v>0</v>
+      </c>
+      <c r="I111" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J111" s="6">
+        <v>0</v>
+      </c>
+      <c r="K111" s="6">
+        <v>0</v>
+      </c>
+      <c r="L111" s="7">
+        <v>0</v>
+      </c>
+      <c r="M111" s="13"/>
+    </row>
+    <row r="112" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A112" s="13"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="13"/>
+      <c r="J112" s="13"/>
+      <c r="K112" s="13"/>
+      <c r="L112" s="13"/>
+      <c r="M112" s="13"/>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A114" s="47"/>
+      <c r="B114" s="47"/>
+      <c r="C114" s="47"/>
+      <c r="D114" s="47"/>
+      <c r="E114" s="47"/>
+      <c r="F114" s="47"/>
+      <c r="G114" s="47"/>
+      <c r="H114" s="47"/>
+      <c r="I114" s="47"/>
+      <c r="J114" s="47"/>
+      <c r="K114" s="47"/>
+      <c r="L114" s="47"/>
+      <c r="M114" s="47"/>
+    </row>
+    <row r="115" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="25">
+        <v>0</v>
+      </c>
+      <c r="B115" s="26"/>
+      <c r="C115" s="26"/>
+      <c r="D115" s="26"/>
+      <c r="E115" s="26"/>
+      <c r="F115" s="26"/>
+      <c r="G115" s="26"/>
+      <c r="H115" s="26"/>
+      <c r="I115" s="26"/>
+      <c r="J115" s="26"/>
+      <c r="K115" s="26"/>
+      <c r="L115" s="27"/>
+      <c r="M115" s="47"/>
+      <c r="O115" s="30"/>
+      <c r="P115" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A116" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="B116" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="C116" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D116" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="E116" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F116" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="G116" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="H116" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="I116" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J116" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="K116" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="L116" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="M116" s="47"/>
+    </row>
+    <row r="117" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A117" s="20">
+        <v>250</v>
+      </c>
+      <c r="B117" s="4">
+        <v>100</v>
+      </c>
+      <c r="C117" s="4">
+        <v>0</v>
+      </c>
+      <c r="D117" s="5">
+        <v>0</v>
+      </c>
+      <c r="E117" s="20">
+        <v>250</v>
+      </c>
+      <c r="F117" s="4">
+        <v>100</v>
+      </c>
+      <c r="G117" s="4">
+        <v>0</v>
+      </c>
+      <c r="H117" s="5">
+        <v>0</v>
+      </c>
+      <c r="I117" s="20">
+        <v>250</v>
+      </c>
+      <c r="J117" s="4">
+        <v>100</v>
+      </c>
+      <c r="K117" s="4">
+        <v>0</v>
+      </c>
+      <c r="L117" s="5">
+        <v>0</v>
+      </c>
+      <c r="M117" s="47"/>
+    </row>
+    <row r="118" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A118" s="20">
+        <v>500</v>
+      </c>
+      <c r="B118" s="4">
+        <v>0</v>
+      </c>
+      <c r="C118" s="4">
+        <v>0</v>
+      </c>
+      <c r="D118" s="5">
+        <v>0</v>
+      </c>
+      <c r="E118" s="20">
+        <v>500</v>
+      </c>
+      <c r="F118" s="4">
+        <v>0</v>
+      </c>
+      <c r="G118" s="4">
+        <v>0</v>
+      </c>
+      <c r="H118" s="5">
+        <v>0</v>
+      </c>
+      <c r="I118" s="20">
+        <v>500</v>
+      </c>
+      <c r="J118" s="4">
+        <v>0</v>
+      </c>
+      <c r="K118" s="4">
+        <v>0</v>
+      </c>
+      <c r="L118" s="5">
+        <v>0</v>
+      </c>
+      <c r="M118" s="47"/>
+    </row>
+    <row r="119" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A119" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B119" s="6">
+        <v>0</v>
+      </c>
+      <c r="C119" s="6">
+        <v>0</v>
+      </c>
+      <c r="D119" s="7">
+        <v>0</v>
+      </c>
+      <c r="E119" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F119" s="6">
+        <v>0</v>
+      </c>
+      <c r="G119" s="6">
+        <v>0</v>
+      </c>
+      <c r="H119" s="7">
+        <v>0</v>
+      </c>
+      <c r="I119" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J119" s="6">
+        <v>0</v>
+      </c>
+      <c r="K119" s="6">
+        <v>0</v>
+      </c>
+      <c r="L119" s="7">
+        <v>0</v>
+      </c>
+      <c r="M119" s="47"/>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M120" s="47"/>
+    </row>
+    <row r="121" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="25">
+        <v>1</v>
+      </c>
+      <c r="B121" s="26"/>
+      <c r="C121" s="26"/>
+      <c r="D121" s="26"/>
+      <c r="E121" s="26"/>
+      <c r="F121" s="26"/>
+      <c r="G121" s="26"/>
+      <c r="H121" s="26"/>
+      <c r="I121" s="26"/>
+      <c r="J121" s="26"/>
+      <c r="K121" s="26"/>
+      <c r="L121" s="27"/>
+      <c r="M121" s="47"/>
+    </row>
+    <row r="122" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A122" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="B122" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="C122" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D122" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="E122" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F122" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="G122" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="H122" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="I122" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J122" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="K122" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="L122" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="M122" s="47"/>
+    </row>
+    <row r="123" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A123" s="20">
+        <v>250</v>
+      </c>
+      <c r="B123" s="4">
+        <v>100</v>
+      </c>
+      <c r="C123" s="4">
+        <v>0</v>
+      </c>
+      <c r="D123" s="5">
+        <v>0</v>
+      </c>
+      <c r="E123" s="20">
+        <v>250</v>
+      </c>
+      <c r="F123" s="4">
+        <v>100</v>
+      </c>
+      <c r="G123" s="4">
+        <v>0</v>
+      </c>
+      <c r="H123" s="5">
+        <v>0</v>
+      </c>
+      <c r="I123" s="20">
+        <v>250</v>
+      </c>
+      <c r="J123" s="4">
+        <v>100</v>
+      </c>
+      <c r="K123" s="4">
+        <v>0</v>
+      </c>
+      <c r="L123" s="5">
+        <v>0</v>
+      </c>
+      <c r="M123" s="47"/>
+    </row>
+    <row r="124" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A124" s="20">
+        <v>500</v>
+      </c>
+      <c r="B124" s="4">
+        <v>0</v>
+      </c>
+      <c r="C124" s="4">
+        <v>0</v>
+      </c>
+      <c r="D124" s="5">
+        <v>0</v>
+      </c>
+      <c r="E124" s="20">
+        <v>500</v>
+      </c>
+      <c r="F124" s="4">
+        <v>0</v>
+      </c>
+      <c r="G124" s="4">
+        <v>0</v>
+      </c>
+      <c r="H124" s="5">
+        <v>0</v>
+      </c>
+      <c r="I124" s="20">
+        <v>500</v>
+      </c>
+      <c r="J124" s="4">
+        <v>0</v>
+      </c>
+      <c r="K124" s="4">
+        <v>0</v>
+      </c>
+      <c r="L124" s="5">
+        <v>0</v>
+      </c>
+      <c r="M124" s="47"/>
+    </row>
+    <row r="125" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A125" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B125" s="6">
+        <v>0</v>
+      </c>
+      <c r="C125" s="6">
+        <v>0</v>
+      </c>
+      <c r="D125" s="7">
+        <v>0</v>
+      </c>
+      <c r="E125" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F125" s="6">
+        <v>0</v>
+      </c>
+      <c r="G125" s="6">
+        <v>0</v>
+      </c>
+      <c r="H125" s="7">
+        <v>0</v>
+      </c>
+      <c r="I125" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J125" s="6">
+        <v>0</v>
+      </c>
+      <c r="K125" s="6">
+        <v>0</v>
+      </c>
+      <c r="L125" s="7">
+        <v>0</v>
+      </c>
+      <c r="M125" s="47"/>
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A126" s="47"/>
+      <c r="B126" s="47"/>
+      <c r="C126" s="47"/>
+      <c r="D126" s="47"/>
+      <c r="E126" s="47"/>
+      <c r="F126" s="47"/>
+      <c r="G126" s="47"/>
+      <c r="H126" s="47"/>
+      <c r="I126" s="47"/>
+      <c r="J126" s="47"/>
+      <c r="K126" s="47"/>
+      <c r="L126" s="47"/>
+      <c r="M126" s="47"/>
+    </row>
+    <row r="127" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A127" s="33"/>
+      <c r="B127" s="34"/>
+      <c r="C127" s="34"/>
+      <c r="D127" s="34"/>
+      <c r="E127" s="35"/>
+      <c r="F127" s="34"/>
+      <c r="G127" s="34"/>
+      <c r="H127" s="34"/>
+      <c r="I127" s="35"/>
+      <c r="J127" s="34"/>
+      <c r="K127" s="34"/>
+      <c r="L127" s="34"/>
+      <c r="M127" s="32"/>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A128" s="48"/>
+      <c r="B128" s="48"/>
+      <c r="C128" s="48"/>
+      <c r="D128" s="48"/>
+      <c r="E128" s="48"/>
+      <c r="F128" s="48"/>
+      <c r="G128" s="48"/>
+      <c r="H128" s="48"/>
+      <c r="I128" s="48"/>
+      <c r="J128" s="48"/>
+      <c r="K128" s="48"/>
+      <c r="L128" s="48"/>
+      <c r="M128" s="48"/>
+    </row>
+    <row r="129" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A129" s="25">
+        <v>0</v>
+      </c>
+      <c r="B129" s="26"/>
+      <c r="C129" s="26"/>
+      <c r="D129" s="26"/>
+      <c r="E129" s="26"/>
+      <c r="F129" s="26"/>
+      <c r="G129" s="26"/>
+      <c r="H129" s="26"/>
+      <c r="I129" s="26"/>
+      <c r="J129" s="26"/>
+      <c r="K129" s="26"/>
+      <c r="L129" s="46"/>
+      <c r="M129" s="48"/>
+      <c r="O129" s="14"/>
+      <c r="P129" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A130" s="37">
+        <v>0.25</v>
+      </c>
+      <c r="B130" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="C130" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="D130" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="E130" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="F130" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="G130" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="H130" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="I130" s="39">
+        <v>0.75</v>
+      </c>
+      <c r="J130" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="K130" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="L130" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="M130" s="48"/>
+    </row>
+    <row r="131" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A131" s="40">
+        <v>250</v>
+      </c>
+      <c r="B131" s="41">
+        <v>97</v>
+      </c>
+      <c r="C131" s="41">
+        <v>0</v>
+      </c>
+      <c r="D131" s="42">
+        <v>0</v>
+      </c>
+      <c r="E131" s="38">
+        <v>250</v>
+      </c>
+      <c r="F131" s="41">
+        <v>98</v>
+      </c>
+      <c r="G131" s="41">
+        <v>0</v>
+      </c>
+      <c r="H131" s="42">
+        <v>0</v>
+      </c>
+      <c r="I131" s="38">
+        <v>250</v>
+      </c>
+      <c r="J131" s="41">
+        <v>96.2</v>
+      </c>
+      <c r="K131" s="41">
+        <v>0</v>
+      </c>
+      <c r="L131" s="42">
+        <v>0</v>
+      </c>
+      <c r="M131" s="48"/>
+    </row>
+    <row r="132" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A132" s="40">
+        <v>500</v>
+      </c>
+      <c r="B132" s="41">
+        <v>97</v>
+      </c>
+      <c r="C132" s="41">
+        <v>0</v>
+      </c>
+      <c r="D132" s="42">
+        <v>0</v>
+      </c>
+      <c r="E132" s="38">
+        <v>500</v>
+      </c>
+      <c r="F132" s="41">
+        <v>97</v>
+      </c>
+      <c r="G132" s="41">
+        <v>0</v>
+      </c>
+      <c r="H132" s="42">
+        <v>0</v>
+      </c>
+      <c r="I132" s="38">
+        <v>500</v>
+      </c>
+      <c r="J132" s="41">
+        <v>96.4</v>
+      </c>
+      <c r="K132" s="41">
+        <v>0</v>
+      </c>
+      <c r="L132" s="42">
+        <v>0</v>
+      </c>
+      <c r="M132" s="48"/>
+    </row>
+    <row r="133" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A133" s="40">
+        <v>1000</v>
+      </c>
+      <c r="B133" s="43">
+        <v>99.4</v>
+      </c>
+      <c r="C133" s="43">
+        <v>0</v>
+      </c>
+      <c r="D133" s="44">
+        <v>0</v>
+      </c>
+      <c r="E133" s="38">
+        <v>1000</v>
+      </c>
+      <c r="F133" s="43">
+        <v>99.6</v>
+      </c>
+      <c r="G133" s="43">
+        <v>0</v>
+      </c>
+      <c r="H133" s="44">
+        <v>0</v>
+      </c>
+      <c r="I133" s="38">
+        <v>1000</v>
+      </c>
+      <c r="J133" s="43">
+        <v>99.8</v>
+      </c>
+      <c r="K133" s="43">
+        <v>0</v>
+      </c>
+      <c r="L133" s="44">
+        <v>0</v>
+      </c>
+      <c r="M133" s="48"/>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A134" s="36"/>
+      <c r="B134" s="36"/>
+      <c r="C134" s="36"/>
+      <c r="D134" s="36"/>
+      <c r="E134" s="36"/>
+      <c r="F134" s="36"/>
+      <c r="G134" s="36"/>
+      <c r="H134" s="36"/>
+      <c r="I134" s="36"/>
+      <c r="J134" s="36"/>
+      <c r="K134" s="36"/>
+      <c r="L134" s="36"/>
+      <c r="M134" s="48"/>
+    </row>
+    <row r="135" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A135" s="25">
+        <v>1</v>
+      </c>
+      <c r="B135" s="26"/>
+      <c r="C135" s="26"/>
+      <c r="D135" s="26"/>
+      <c r="E135" s="26"/>
+      <c r="F135" s="26"/>
+      <c r="G135" s="26"/>
+      <c r="H135" s="26"/>
+      <c r="I135" s="26"/>
+      <c r="J135" s="26"/>
+      <c r="K135" s="26"/>
+      <c r="L135" s="46"/>
+      <c r="M135" s="48"/>
+    </row>
+    <row r="136" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A136" s="45">
+        <v>0.25</v>
+      </c>
+      <c r="B136" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="C136" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="D136" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="E136" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="F136" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="G136" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="H136" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="I136" s="39">
+        <v>0.75</v>
+      </c>
+      <c r="J136" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="K136" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="L136" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="M136" s="48"/>
+    </row>
+    <row r="137" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A137" s="40">
+        <v>250</v>
+      </c>
+      <c r="B137" s="41">
+        <v>96.2</v>
+      </c>
+      <c r="C137" s="41">
+        <v>0</v>
+      </c>
+      <c r="D137" s="42">
+        <v>0</v>
+      </c>
+      <c r="E137" s="38">
+        <v>250</v>
+      </c>
+      <c r="F137" s="41">
+        <v>98.2</v>
+      </c>
+      <c r="G137" s="41">
+        <v>0</v>
+      </c>
+      <c r="H137" s="42">
+        <v>0</v>
+      </c>
+      <c r="I137" s="38">
+        <v>250</v>
+      </c>
+      <c r="J137" s="41">
+        <v>99.6</v>
+      </c>
+      <c r="K137" s="41">
+        <v>0</v>
+      </c>
+      <c r="L137" s="42">
+        <v>0</v>
+      </c>
+      <c r="M137" s="48"/>
+    </row>
+    <row r="138" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A138" s="40">
+        <v>500</v>
+      </c>
+      <c r="B138" s="41">
+        <v>96.4</v>
+      </c>
+      <c r="C138" s="41">
+        <v>0</v>
+      </c>
+      <c r="D138" s="42">
+        <v>0</v>
+      </c>
+      <c r="E138" s="38">
+        <v>500</v>
+      </c>
+      <c r="F138" s="41">
+        <v>96.6</v>
+      </c>
+      <c r="G138" s="41">
+        <v>0</v>
+      </c>
+      <c r="H138" s="42">
+        <v>0</v>
+      </c>
+      <c r="I138" s="38">
+        <v>500</v>
+      </c>
+      <c r="J138" s="41">
+        <v>98</v>
+      </c>
+      <c r="K138" s="41">
+        <v>0</v>
+      </c>
+      <c r="L138" s="42">
+        <v>0</v>
+      </c>
+      <c r="M138" s="48"/>
+    </row>
+    <row r="139" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A139" s="40">
+        <v>1000</v>
+      </c>
+      <c r="B139" s="43">
+        <v>99.8</v>
+      </c>
+      <c r="C139" s="43">
+        <v>0</v>
+      </c>
+      <c r="D139" s="44">
+        <v>0</v>
+      </c>
+      <c r="E139" s="38">
+        <v>1000</v>
+      </c>
+      <c r="F139" s="43">
+        <v>100</v>
+      </c>
+      <c r="G139" s="43">
+        <v>0</v>
+      </c>
+      <c r="H139" s="44">
+        <v>0</v>
+      </c>
+      <c r="I139" s="38">
+        <v>1000</v>
+      </c>
+      <c r="J139" s="43">
+        <v>99.8</v>
+      </c>
+      <c r="K139" s="43">
+        <v>0</v>
+      </c>
+      <c r="L139" s="44">
+        <v>0</v>
+      </c>
+      <c r="M139" s="48"/>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A140" s="48"/>
+      <c r="B140" s="48"/>
+      <c r="C140" s="48"/>
+      <c r="D140" s="48"/>
+      <c r="E140" s="48"/>
+      <c r="F140" s="48"/>
+      <c r="G140" s="48"/>
+      <c r="H140" s="48"/>
+      <c r="I140" s="48"/>
+      <c r="J140" s="48"/>
+      <c r="K140" s="48"/>
+      <c r="L140" s="48"/>
+      <c r="M140" s="48"/>
+    </row>
   </sheetData>
-  <mergeCells count="68">
+  <mergeCells count="74">
+    <mergeCell ref="A135:L135"/>
+    <mergeCell ref="A115:L115"/>
+    <mergeCell ref="A121:L121"/>
+    <mergeCell ref="A129:L129"/>
+    <mergeCell ref="A101:L101"/>
+    <mergeCell ref="A107:L107"/>
     <mergeCell ref="M88:N88"/>
     <mergeCell ref="P88:Q88"/>
     <mergeCell ref="R88:S88"/>

</xml_diff>

<commit_message>
Adding new effect size conditions
</commit_message>
<xml_diff>
--- a/Sim_DataFrame_Plan.xlsx
+++ b/Sim_DataFrame_Plan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conorlacey/Documents/Grad School/Research/Thesis/Thesis R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D6827D-3346-E344-A7D9-B4B5F25A7D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD74CD7-5B3F-9643-9D2E-D3478BB07938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2CE5E951-8CB5-3C4B-AF22-C52294E8CEFF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{2CE5E951-8CB5-3C4B-AF22-C52294E8CEFF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Small Effects" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Each cell will be the mean estimate after 500 replications.</t>
   </si>
@@ -751,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DB3B1C-C16F-EB40-8F32-8665E0986627}">
   <dimension ref="A1:Y140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="75" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="M139" sqref="M139"/>
+    <sheetView topLeftCell="A119" zoomScale="75" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="Q141" sqref="A100:Q141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5304,4 +5305,2346 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A29300A-14B0-A04E-B5B1-9DF5E58F3BCD}">
+  <dimension ref="A1:P84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="75" workbookViewId="0">
+      <selection activeCell="T66" sqref="T66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+    </row>
+    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="25">
+        <v>0</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="B3" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H3" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J3" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K3" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L3" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M3" s="13"/>
+    </row>
+    <row r="4" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
+        <v>250</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5">
+        <v>7</v>
+      </c>
+      <c r="E4" s="20">
+        <v>250</v>
+      </c>
+      <c r="F4" s="4">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5">
+        <v>16</v>
+      </c>
+      <c r="I4" s="20">
+        <v>250</v>
+      </c>
+      <c r="J4" s="4">
+        <v>19</v>
+      </c>
+      <c r="K4" s="4">
+        <v>22</v>
+      </c>
+      <c r="L4" s="5">
+        <v>25</v>
+      </c>
+      <c r="M4" s="13"/>
+    </row>
+    <row r="5" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
+        <v>500</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="20">
+        <v>500</v>
+      </c>
+      <c r="F5" s="4">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4">
+        <v>14</v>
+      </c>
+      <c r="H5" s="5">
+        <v>17</v>
+      </c>
+      <c r="I5" s="20">
+        <v>500</v>
+      </c>
+      <c r="J5" s="4">
+        <v>20</v>
+      </c>
+      <c r="K5" s="4">
+        <v>23</v>
+      </c>
+      <c r="L5" s="5">
+        <v>26</v>
+      </c>
+      <c r="M5" s="13"/>
+    </row>
+    <row r="6" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7">
+        <v>9</v>
+      </c>
+      <c r="E6" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F6" s="6">
+        <v>12</v>
+      </c>
+      <c r="G6" s="6">
+        <v>15</v>
+      </c>
+      <c r="H6" s="7">
+        <v>18</v>
+      </c>
+      <c r="I6" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J6" s="6">
+        <v>21</v>
+      </c>
+      <c r="K6" s="6">
+        <v>24</v>
+      </c>
+      <c r="L6" s="7">
+        <v>27</v>
+      </c>
+      <c r="M6" s="13"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
+        <v>1</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="13"/>
+    </row>
+    <row r="9" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="B9" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H9" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J9" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K9" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L9" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M9" s="13"/>
+    </row>
+    <row r="10" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="20">
+        <v>250</v>
+      </c>
+      <c r="B10" s="4">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5">
+        <v>34</v>
+      </c>
+      <c r="E10" s="20">
+        <v>250</v>
+      </c>
+      <c r="F10" s="4">
+        <v>37</v>
+      </c>
+      <c r="G10" s="4">
+        <v>40</v>
+      </c>
+      <c r="H10" s="5">
+        <v>43</v>
+      </c>
+      <c r="I10" s="20">
+        <v>250</v>
+      </c>
+      <c r="J10" s="4">
+        <v>46</v>
+      </c>
+      <c r="K10" s="4">
+        <v>49</v>
+      </c>
+      <c r="L10" s="5">
+        <v>52</v>
+      </c>
+      <c r="M10" s="13"/>
+    </row>
+    <row r="11" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>500</v>
+      </c>
+      <c r="B11" s="4">
+        <v>29</v>
+      </c>
+      <c r="C11" s="4">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5">
+        <v>35</v>
+      </c>
+      <c r="E11" s="20">
+        <v>500</v>
+      </c>
+      <c r="F11" s="4">
+        <v>38</v>
+      </c>
+      <c r="G11" s="4">
+        <v>41</v>
+      </c>
+      <c r="H11" s="5">
+        <v>44</v>
+      </c>
+      <c r="I11" s="20">
+        <v>500</v>
+      </c>
+      <c r="J11" s="4">
+        <v>47</v>
+      </c>
+      <c r="K11" s="4">
+        <v>50</v>
+      </c>
+      <c r="L11" s="5">
+        <v>53</v>
+      </c>
+      <c r="M11" s="13"/>
+    </row>
+    <row r="12" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B12" s="6">
+        <v>30</v>
+      </c>
+      <c r="C12" s="6">
+        <v>33</v>
+      </c>
+      <c r="D12" s="7">
+        <v>36</v>
+      </c>
+      <c r="E12" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F12" s="6">
+        <v>39</v>
+      </c>
+      <c r="G12" s="6">
+        <v>42</v>
+      </c>
+      <c r="H12" s="7">
+        <v>45</v>
+      </c>
+      <c r="I12" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J12" s="6">
+        <v>48</v>
+      </c>
+      <c r="K12" s="6">
+        <v>51</v>
+      </c>
+      <c r="L12" s="7">
+        <v>54</v>
+      </c>
+      <c r="M12" s="13"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+    </row>
+    <row r="16" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="25">
+        <v>0</v>
+      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="B17" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C17" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H17" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J17" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K17" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L17" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M17" s="30"/>
+    </row>
+    <row r="18" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
+        <v>250</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5">
+        <v>7</v>
+      </c>
+      <c r="E18" s="20">
+        <v>250</v>
+      </c>
+      <c r="F18" s="4">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4">
+        <v>13</v>
+      </c>
+      <c r="H18" s="5">
+        <v>16</v>
+      </c>
+      <c r="I18" s="20">
+        <v>250</v>
+      </c>
+      <c r="J18" s="4">
+        <v>19</v>
+      </c>
+      <c r="K18" s="4">
+        <v>22</v>
+      </c>
+      <c r="L18" s="5">
+        <v>25</v>
+      </c>
+      <c r="M18" s="30"/>
+    </row>
+    <row r="19" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>500</v>
+      </c>
+      <c r="B19" s="4">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4">
+        <v>5</v>
+      </c>
+      <c r="D19" s="5">
+        <v>8</v>
+      </c>
+      <c r="E19" s="20">
+        <v>500</v>
+      </c>
+      <c r="F19" s="4">
+        <v>11</v>
+      </c>
+      <c r="G19" s="4">
+        <v>14</v>
+      </c>
+      <c r="H19" s="5">
+        <v>17</v>
+      </c>
+      <c r="I19" s="20">
+        <v>500</v>
+      </c>
+      <c r="J19" s="4">
+        <v>20</v>
+      </c>
+      <c r="K19" s="4">
+        <v>23</v>
+      </c>
+      <c r="L19" s="5">
+        <v>26</v>
+      </c>
+      <c r="M19" s="30"/>
+    </row>
+    <row r="20" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B20" s="6">
+        <v>3</v>
+      </c>
+      <c r="C20" s="6">
+        <v>6</v>
+      </c>
+      <c r="D20" s="7">
+        <v>9</v>
+      </c>
+      <c r="E20" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F20" s="6">
+        <v>12</v>
+      </c>
+      <c r="G20" s="6">
+        <v>15</v>
+      </c>
+      <c r="H20" s="7">
+        <v>18</v>
+      </c>
+      <c r="I20" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J20" s="6">
+        <v>21</v>
+      </c>
+      <c r="K20" s="6">
+        <v>24</v>
+      </c>
+      <c r="L20" s="7">
+        <v>27</v>
+      </c>
+      <c r="M20" s="30"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M21" s="30"/>
+    </row>
+    <row r="22" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
+        <v>1</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="30"/>
+    </row>
+    <row r="23" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="B23" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C23" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F23" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G23" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H23" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I23" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J23" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K23" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L23" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M23" s="30"/>
+    </row>
+    <row r="24" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" s="20">
+        <v>250</v>
+      </c>
+      <c r="B24" s="4">
+        <v>28</v>
+      </c>
+      <c r="C24" s="4">
+        <v>31</v>
+      </c>
+      <c r="D24" s="5">
+        <v>34</v>
+      </c>
+      <c r="E24" s="20">
+        <v>250</v>
+      </c>
+      <c r="F24" s="4">
+        <v>37</v>
+      </c>
+      <c r="G24" s="4">
+        <v>40</v>
+      </c>
+      <c r="H24" s="5">
+        <v>43</v>
+      </c>
+      <c r="I24" s="20">
+        <v>250</v>
+      </c>
+      <c r="J24" s="4">
+        <v>46</v>
+      </c>
+      <c r="K24" s="4">
+        <v>49</v>
+      </c>
+      <c r="L24" s="5">
+        <v>52</v>
+      </c>
+      <c r="M24" s="30"/>
+    </row>
+    <row r="25" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
+        <v>500</v>
+      </c>
+      <c r="B25" s="4">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4">
+        <v>32</v>
+      </c>
+      <c r="D25" s="5">
+        <v>35</v>
+      </c>
+      <c r="E25" s="20">
+        <v>500</v>
+      </c>
+      <c r="F25" s="4">
+        <v>38</v>
+      </c>
+      <c r="G25" s="4">
+        <v>41</v>
+      </c>
+      <c r="H25" s="5">
+        <v>44</v>
+      </c>
+      <c r="I25" s="20">
+        <v>500</v>
+      </c>
+      <c r="J25" s="4">
+        <v>47</v>
+      </c>
+      <c r="K25" s="4">
+        <v>50</v>
+      </c>
+      <c r="L25" s="5">
+        <v>53</v>
+      </c>
+      <c r="M25" s="30"/>
+    </row>
+    <row r="26" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B26" s="6">
+        <v>30</v>
+      </c>
+      <c r="C26" s="6">
+        <v>33</v>
+      </c>
+      <c r="D26" s="7">
+        <v>36</v>
+      </c>
+      <c r="E26" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F26" s="6">
+        <v>39</v>
+      </c>
+      <c r="G26" s="6">
+        <v>42</v>
+      </c>
+      <c r="H26" s="7">
+        <v>45</v>
+      </c>
+      <c r="I26" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J26" s="6">
+        <v>48</v>
+      </c>
+      <c r="K26" s="6">
+        <v>51</v>
+      </c>
+      <c r="L26" s="7">
+        <v>54</v>
+      </c>
+      <c r="M26" s="30"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+    </row>
+    <row r="30" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="25">
+        <v>0</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="B31" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C31" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D31" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E31" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G31" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H31" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I31" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J31" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K31" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L31" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M31" s="14"/>
+    </row>
+    <row r="32" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A32" s="20">
+        <v>250</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4">
+        <v>4</v>
+      </c>
+      <c r="D32" s="5">
+        <v>7</v>
+      </c>
+      <c r="E32" s="20">
+        <v>250</v>
+      </c>
+      <c r="F32" s="4">
+        <v>10</v>
+      </c>
+      <c r="G32" s="4">
+        <v>13</v>
+      </c>
+      <c r="H32" s="5">
+        <v>16</v>
+      </c>
+      <c r="I32" s="20">
+        <v>250</v>
+      </c>
+      <c r="J32" s="4">
+        <v>19</v>
+      </c>
+      <c r="K32" s="4">
+        <v>22</v>
+      </c>
+      <c r="L32" s="5">
+        <v>25</v>
+      </c>
+      <c r="M32" s="14"/>
+    </row>
+    <row r="33" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="20">
+        <v>500</v>
+      </c>
+      <c r="B33" s="4">
+        <v>2</v>
+      </c>
+      <c r="C33" s="4">
+        <v>5</v>
+      </c>
+      <c r="D33" s="5">
+        <v>8</v>
+      </c>
+      <c r="E33" s="20">
+        <v>500</v>
+      </c>
+      <c r="F33" s="4">
+        <v>11</v>
+      </c>
+      <c r="G33" s="4">
+        <v>14</v>
+      </c>
+      <c r="H33" s="5">
+        <v>17</v>
+      </c>
+      <c r="I33" s="20">
+        <v>500</v>
+      </c>
+      <c r="J33" s="4">
+        <v>20</v>
+      </c>
+      <c r="K33" s="4">
+        <v>23</v>
+      </c>
+      <c r="L33" s="5">
+        <v>26</v>
+      </c>
+      <c r="M33" s="14"/>
+    </row>
+    <row r="34" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B34" s="6">
+        <v>3</v>
+      </c>
+      <c r="C34" s="6">
+        <v>6</v>
+      </c>
+      <c r="D34" s="7">
+        <v>9</v>
+      </c>
+      <c r="E34" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F34" s="6">
+        <v>12</v>
+      </c>
+      <c r="G34" s="6">
+        <v>15</v>
+      </c>
+      <c r="H34" s="7">
+        <v>18</v>
+      </c>
+      <c r="I34" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J34" s="6">
+        <v>21</v>
+      </c>
+      <c r="K34" s="6">
+        <v>24</v>
+      </c>
+      <c r="L34" s="7">
+        <v>27</v>
+      </c>
+      <c r="M34" s="14"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M35" s="14"/>
+    </row>
+    <row r="36" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="25">
+        <v>1</v>
+      </c>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="14"/>
+    </row>
+    <row r="37" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="B37" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C37" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D37" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F37" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G37" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H37" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I37" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J37" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K37" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L37" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M37" s="14"/>
+    </row>
+    <row r="38" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A38" s="20">
+        <v>250</v>
+      </c>
+      <c r="B38" s="4">
+        <v>28</v>
+      </c>
+      <c r="C38" s="4">
+        <v>31</v>
+      </c>
+      <c r="D38" s="5">
+        <v>34</v>
+      </c>
+      <c r="E38" s="20">
+        <v>250</v>
+      </c>
+      <c r="F38" s="4">
+        <v>37</v>
+      </c>
+      <c r="G38" s="4">
+        <v>40</v>
+      </c>
+      <c r="H38" s="5">
+        <v>43</v>
+      </c>
+      <c r="I38" s="20">
+        <v>250</v>
+      </c>
+      <c r="J38" s="4">
+        <v>46</v>
+      </c>
+      <c r="K38" s="4">
+        <v>49</v>
+      </c>
+      <c r="L38" s="5">
+        <v>52</v>
+      </c>
+      <c r="M38" s="14"/>
+    </row>
+    <row r="39" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="20">
+        <v>500</v>
+      </c>
+      <c r="B39" s="4">
+        <v>29</v>
+      </c>
+      <c r="C39" s="4">
+        <v>32</v>
+      </c>
+      <c r="D39" s="5">
+        <v>35</v>
+      </c>
+      <c r="E39" s="20">
+        <v>500</v>
+      </c>
+      <c r="F39" s="4">
+        <v>38</v>
+      </c>
+      <c r="G39" s="4">
+        <v>41</v>
+      </c>
+      <c r="H39" s="5">
+        <v>44</v>
+      </c>
+      <c r="I39" s="20">
+        <v>500</v>
+      </c>
+      <c r="J39" s="4">
+        <v>47</v>
+      </c>
+      <c r="K39" s="4">
+        <v>50</v>
+      </c>
+      <c r="L39" s="5">
+        <v>53</v>
+      </c>
+      <c r="M39" s="14"/>
+    </row>
+    <row r="40" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B40" s="6">
+        <v>30</v>
+      </c>
+      <c r="C40" s="6">
+        <v>33</v>
+      </c>
+      <c r="D40" s="7">
+        <v>36</v>
+      </c>
+      <c r="E40" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F40" s="6">
+        <v>39</v>
+      </c>
+      <c r="G40" s="6">
+        <v>42</v>
+      </c>
+      <c r="H40" s="7">
+        <v>45</v>
+      </c>
+      <c r="I40" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J40" s="6">
+        <v>48</v>
+      </c>
+      <c r="K40" s="6">
+        <v>51</v>
+      </c>
+      <c r="L40" s="7">
+        <v>54</v>
+      </c>
+      <c r="M40" s="14"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+    </row>
+    <row r="45" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A45" s="25">
+        <v>0</v>
+      </c>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="13"/>
+      <c r="O45" s="13"/>
+      <c r="P45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="B46" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C46" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D46" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E46" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F46" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G46" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H46" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I46" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J46" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K46" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L46" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M46" s="13"/>
+    </row>
+    <row r="47" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A47" s="20">
+        <v>250</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+      <c r="C47" s="4">
+        <v>4</v>
+      </c>
+      <c r="D47" s="5">
+        <v>7</v>
+      </c>
+      <c r="E47" s="20">
+        <v>250</v>
+      </c>
+      <c r="F47" s="4">
+        <v>10</v>
+      </c>
+      <c r="G47" s="4">
+        <v>13</v>
+      </c>
+      <c r="H47" s="5">
+        <v>16</v>
+      </c>
+      <c r="I47" s="20">
+        <v>250</v>
+      </c>
+      <c r="J47" s="4">
+        <v>19</v>
+      </c>
+      <c r="K47" s="4">
+        <v>22</v>
+      </c>
+      <c r="L47" s="5">
+        <v>25</v>
+      </c>
+      <c r="M47" s="13"/>
+    </row>
+    <row r="48" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A48" s="20">
+        <v>500</v>
+      </c>
+      <c r="B48" s="4">
+        <v>2</v>
+      </c>
+      <c r="C48" s="4">
+        <v>5</v>
+      </c>
+      <c r="D48" s="5">
+        <v>8</v>
+      </c>
+      <c r="E48" s="20">
+        <v>500</v>
+      </c>
+      <c r="F48" s="4">
+        <v>11</v>
+      </c>
+      <c r="G48" s="4">
+        <v>14</v>
+      </c>
+      <c r="H48" s="5">
+        <v>17</v>
+      </c>
+      <c r="I48" s="20">
+        <v>500</v>
+      </c>
+      <c r="J48" s="4">
+        <v>20</v>
+      </c>
+      <c r="K48" s="4">
+        <v>23</v>
+      </c>
+      <c r="L48" s="5">
+        <v>26</v>
+      </c>
+      <c r="M48" s="13"/>
+    </row>
+    <row r="49" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A49" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B49" s="6">
+        <v>3</v>
+      </c>
+      <c r="C49" s="6">
+        <v>6</v>
+      </c>
+      <c r="D49" s="7">
+        <v>9</v>
+      </c>
+      <c r="E49" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F49" s="6">
+        <v>12</v>
+      </c>
+      <c r="G49" s="6">
+        <v>15</v>
+      </c>
+      <c r="H49" s="7">
+        <v>18</v>
+      </c>
+      <c r="I49" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J49" s="6">
+        <v>21</v>
+      </c>
+      <c r="K49" s="6">
+        <v>24</v>
+      </c>
+      <c r="L49" s="7">
+        <v>27</v>
+      </c>
+      <c r="M49" s="13"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M50" s="13"/>
+    </row>
+    <row r="51" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A51" s="25">
+        <v>1</v>
+      </c>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="27"/>
+      <c r="M51" s="13"/>
+    </row>
+    <row r="52" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="B52" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C52" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D52" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E52" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F52" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G52" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H52" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I52" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J52" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K52" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L52" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M52" s="13"/>
+    </row>
+    <row r="53" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A53" s="20">
+        <v>250</v>
+      </c>
+      <c r="B53" s="4">
+        <v>28</v>
+      </c>
+      <c r="C53" s="4">
+        <v>31</v>
+      </c>
+      <c r="D53" s="5">
+        <v>34</v>
+      </c>
+      <c r="E53" s="20">
+        <v>250</v>
+      </c>
+      <c r="F53" s="4">
+        <v>37</v>
+      </c>
+      <c r="G53" s="4">
+        <v>40</v>
+      </c>
+      <c r="H53" s="5">
+        <v>43</v>
+      </c>
+      <c r="I53" s="20">
+        <v>250</v>
+      </c>
+      <c r="J53" s="4">
+        <v>46</v>
+      </c>
+      <c r="K53" s="4">
+        <v>49</v>
+      </c>
+      <c r="L53" s="5">
+        <v>52</v>
+      </c>
+      <c r="M53" s="13"/>
+    </row>
+    <row r="54" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A54" s="20">
+        <v>500</v>
+      </c>
+      <c r="B54" s="4">
+        <v>29</v>
+      </c>
+      <c r="C54" s="4">
+        <v>32</v>
+      </c>
+      <c r="D54" s="5">
+        <v>35</v>
+      </c>
+      <c r="E54" s="20">
+        <v>500</v>
+      </c>
+      <c r="F54" s="4">
+        <v>38</v>
+      </c>
+      <c r="G54" s="4">
+        <v>41</v>
+      </c>
+      <c r="H54" s="5">
+        <v>44</v>
+      </c>
+      <c r="I54" s="20">
+        <v>500</v>
+      </c>
+      <c r="J54" s="4">
+        <v>47</v>
+      </c>
+      <c r="K54" s="4">
+        <v>50</v>
+      </c>
+      <c r="L54" s="5">
+        <v>53</v>
+      </c>
+      <c r="M54" s="13"/>
+    </row>
+    <row r="55" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A55" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B55" s="6">
+        <v>30</v>
+      </c>
+      <c r="C55" s="6">
+        <v>33</v>
+      </c>
+      <c r="D55" s="7">
+        <v>36</v>
+      </c>
+      <c r="E55" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F55" s="6">
+        <v>39</v>
+      </c>
+      <c r="G55" s="6">
+        <v>42</v>
+      </c>
+      <c r="H55" s="7">
+        <v>45</v>
+      </c>
+      <c r="I55" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J55" s="6">
+        <v>48</v>
+      </c>
+      <c r="K55" s="6">
+        <v>51</v>
+      </c>
+      <c r="L55" s="7">
+        <v>54</v>
+      </c>
+      <c r="M55" s="13"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="13"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A58" s="47"/>
+      <c r="B58" s="47"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="47"/>
+      <c r="J58" s="47"/>
+      <c r="K58" s="47"/>
+      <c r="L58" s="47"/>
+      <c r="M58" s="47"/>
+    </row>
+    <row r="59" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A59" s="25">
+        <v>0</v>
+      </c>
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="27"/>
+      <c r="M59" s="47"/>
+      <c r="O59" s="30"/>
+      <c r="P59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="B60" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C60" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D60" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E60" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F60" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G60" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H60" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I60" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J60" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K60" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L60" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M60" s="47"/>
+    </row>
+    <row r="61" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A61" s="20">
+        <v>250</v>
+      </c>
+      <c r="B61" s="4">
+        <v>1</v>
+      </c>
+      <c r="C61" s="4">
+        <v>4</v>
+      </c>
+      <c r="D61" s="5">
+        <v>7</v>
+      </c>
+      <c r="E61" s="20">
+        <v>250</v>
+      </c>
+      <c r="F61" s="4">
+        <v>10</v>
+      </c>
+      <c r="G61" s="4">
+        <v>13</v>
+      </c>
+      <c r="H61" s="5">
+        <v>16</v>
+      </c>
+      <c r="I61" s="20">
+        <v>250</v>
+      </c>
+      <c r="J61" s="4">
+        <v>19</v>
+      </c>
+      <c r="K61" s="4">
+        <v>22</v>
+      </c>
+      <c r="L61" s="5">
+        <v>25</v>
+      </c>
+      <c r="M61" s="47"/>
+    </row>
+    <row r="62" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A62" s="20">
+        <v>500</v>
+      </c>
+      <c r="B62" s="4">
+        <v>2</v>
+      </c>
+      <c r="C62" s="4">
+        <v>5</v>
+      </c>
+      <c r="D62" s="5">
+        <v>8</v>
+      </c>
+      <c r="E62" s="20">
+        <v>500</v>
+      </c>
+      <c r="F62" s="4">
+        <v>11</v>
+      </c>
+      <c r="G62" s="4">
+        <v>14</v>
+      </c>
+      <c r="H62" s="5">
+        <v>17</v>
+      </c>
+      <c r="I62" s="20">
+        <v>500</v>
+      </c>
+      <c r="J62" s="4">
+        <v>20</v>
+      </c>
+      <c r="K62" s="4">
+        <v>23</v>
+      </c>
+      <c r="L62" s="5">
+        <v>26</v>
+      </c>
+      <c r="M62" s="47"/>
+    </row>
+    <row r="63" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A63" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B63" s="6">
+        <v>3</v>
+      </c>
+      <c r="C63" s="6">
+        <v>6</v>
+      </c>
+      <c r="D63" s="7">
+        <v>9</v>
+      </c>
+      <c r="E63" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F63" s="6">
+        <v>12</v>
+      </c>
+      <c r="G63" s="6">
+        <v>15</v>
+      </c>
+      <c r="H63" s="7">
+        <v>18</v>
+      </c>
+      <c r="I63" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J63" s="6">
+        <v>21</v>
+      </c>
+      <c r="K63" s="6">
+        <v>24</v>
+      </c>
+      <c r="L63" s="7">
+        <v>27</v>
+      </c>
+      <c r="M63" s="47"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M64" s="47"/>
+    </row>
+    <row r="65" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A65" s="25">
+        <v>1</v>
+      </c>
+      <c r="B65" s="26"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="26"/>
+      <c r="J65" s="26"/>
+      <c r="K65" s="26"/>
+      <c r="L65" s="27"/>
+      <c r="M65" s="47"/>
+    </row>
+    <row r="66" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A66" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="B66" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C66" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D66" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E66" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F66" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G66" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H66" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I66" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J66" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K66" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L66" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M66" s="47"/>
+    </row>
+    <row r="67" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A67" s="20">
+        <v>250</v>
+      </c>
+      <c r="B67" s="4">
+        <v>28</v>
+      </c>
+      <c r="C67" s="4">
+        <v>31</v>
+      </c>
+      <c r="D67" s="5">
+        <v>34</v>
+      </c>
+      <c r="E67" s="20">
+        <v>250</v>
+      </c>
+      <c r="F67" s="4">
+        <v>37</v>
+      </c>
+      <c r="G67" s="4">
+        <v>40</v>
+      </c>
+      <c r="H67" s="5">
+        <v>43</v>
+      </c>
+      <c r="I67" s="20">
+        <v>250</v>
+      </c>
+      <c r="J67" s="4">
+        <v>46</v>
+      </c>
+      <c r="K67" s="4">
+        <v>49</v>
+      </c>
+      <c r="L67" s="5">
+        <v>52</v>
+      </c>
+      <c r="M67" s="47"/>
+    </row>
+    <row r="68" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A68" s="20">
+        <v>500</v>
+      </c>
+      <c r="B68" s="4">
+        <v>29</v>
+      </c>
+      <c r="C68" s="4">
+        <v>32</v>
+      </c>
+      <c r="D68" s="5">
+        <v>35</v>
+      </c>
+      <c r="E68" s="20">
+        <v>500</v>
+      </c>
+      <c r="F68" s="4">
+        <v>38</v>
+      </c>
+      <c r="G68" s="4">
+        <v>41</v>
+      </c>
+      <c r="H68" s="5">
+        <v>44</v>
+      </c>
+      <c r="I68" s="20">
+        <v>500</v>
+      </c>
+      <c r="J68" s="4">
+        <v>47</v>
+      </c>
+      <c r="K68" s="4">
+        <v>50</v>
+      </c>
+      <c r="L68" s="5">
+        <v>53</v>
+      </c>
+      <c r="M68" s="47"/>
+    </row>
+    <row r="69" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A69" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B69" s="6">
+        <v>30</v>
+      </c>
+      <c r="C69" s="6">
+        <v>33</v>
+      </c>
+      <c r="D69" s="7">
+        <v>36</v>
+      </c>
+      <c r="E69" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F69" s="6">
+        <v>39</v>
+      </c>
+      <c r="G69" s="6">
+        <v>42</v>
+      </c>
+      <c r="H69" s="7">
+        <v>45</v>
+      </c>
+      <c r="I69" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J69" s="6">
+        <v>48</v>
+      </c>
+      <c r="K69" s="6">
+        <v>51</v>
+      </c>
+      <c r="L69" s="7">
+        <v>54</v>
+      </c>
+      <c r="M69" s="47"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A70" s="47"/>
+      <c r="B70" s="47"/>
+      <c r="C70" s="47"/>
+      <c r="D70" s="47"/>
+      <c r="E70" s="47"/>
+      <c r="F70" s="47"/>
+      <c r="G70" s="47"/>
+      <c r="H70" s="47"/>
+      <c r="I70" s="47"/>
+      <c r="J70" s="47"/>
+      <c r="K70" s="47"/>
+      <c r="L70" s="47"/>
+      <c r="M70" s="47"/>
+    </row>
+    <row r="71" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A71" s="33"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="35"/>
+      <c r="F71" s="34"/>
+      <c r="G71" s="34"/>
+      <c r="H71" s="34"/>
+      <c r="I71" s="35"/>
+      <c r="J71" s="34"/>
+      <c r="K71" s="34"/>
+      <c r="L71" s="34"/>
+      <c r="M71" s="32"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A72" s="48"/>
+      <c r="B72" s="48"/>
+      <c r="C72" s="48"/>
+      <c r="D72" s="48"/>
+      <c r="E72" s="48"/>
+      <c r="F72" s="48"/>
+      <c r="G72" s="48"/>
+      <c r="H72" s="48"/>
+      <c r="I72" s="48"/>
+      <c r="J72" s="48"/>
+      <c r="K72" s="48"/>
+      <c r="L72" s="48"/>
+      <c r="M72" s="48"/>
+    </row>
+    <row r="73" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A73" s="25">
+        <v>0</v>
+      </c>
+      <c r="B73" s="26"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="26"/>
+      <c r="G73" s="26"/>
+      <c r="H73" s="26"/>
+      <c r="I73" s="26"/>
+      <c r="J73" s="26"/>
+      <c r="K73" s="26"/>
+      <c r="L73" s="27"/>
+      <c r="M73" s="48"/>
+      <c r="O73" s="14"/>
+      <c r="P73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A74" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="B74" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C74" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D74" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E74" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F74" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G74" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H74" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I74" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J74" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K74" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L74" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M74" s="48"/>
+    </row>
+    <row r="75" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A75" s="20">
+        <v>250</v>
+      </c>
+      <c r="B75" s="4">
+        <v>1</v>
+      </c>
+      <c r="C75" s="4">
+        <v>4</v>
+      </c>
+      <c r="D75" s="5">
+        <v>7</v>
+      </c>
+      <c r="E75" s="20">
+        <v>250</v>
+      </c>
+      <c r="F75" s="4">
+        <v>10</v>
+      </c>
+      <c r="G75" s="4">
+        <v>13</v>
+      </c>
+      <c r="H75" s="5">
+        <v>16</v>
+      </c>
+      <c r="I75" s="20">
+        <v>250</v>
+      </c>
+      <c r="J75" s="4">
+        <v>19</v>
+      </c>
+      <c r="K75" s="4">
+        <v>22</v>
+      </c>
+      <c r="L75" s="5">
+        <v>25</v>
+      </c>
+      <c r="M75" s="48"/>
+    </row>
+    <row r="76" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <v>500</v>
+      </c>
+      <c r="B76" s="4">
+        <v>2</v>
+      </c>
+      <c r="C76" s="4">
+        <v>5</v>
+      </c>
+      <c r="D76" s="5">
+        <v>8</v>
+      </c>
+      <c r="E76" s="20">
+        <v>500</v>
+      </c>
+      <c r="F76" s="4">
+        <v>11</v>
+      </c>
+      <c r="G76" s="4">
+        <v>14</v>
+      </c>
+      <c r="H76" s="5">
+        <v>17</v>
+      </c>
+      <c r="I76" s="20">
+        <v>500</v>
+      </c>
+      <c r="J76" s="4">
+        <v>20</v>
+      </c>
+      <c r="K76" s="4">
+        <v>23</v>
+      </c>
+      <c r="L76" s="5">
+        <v>26</v>
+      </c>
+      <c r="M76" s="48"/>
+    </row>
+    <row r="77" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B77" s="6">
+        <v>3</v>
+      </c>
+      <c r="C77" s="6">
+        <v>6</v>
+      </c>
+      <c r="D77" s="7">
+        <v>9</v>
+      </c>
+      <c r="E77" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F77" s="6">
+        <v>12</v>
+      </c>
+      <c r="G77" s="6">
+        <v>15</v>
+      </c>
+      <c r="H77" s="7">
+        <v>18</v>
+      </c>
+      <c r="I77" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J77" s="6">
+        <v>21</v>
+      </c>
+      <c r="K77" s="6">
+        <v>24</v>
+      </c>
+      <c r="L77" s="7">
+        <v>27</v>
+      </c>
+      <c r="M77" s="48"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M78" s="48"/>
+    </row>
+    <row r="79" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A79" s="25">
+        <v>1</v>
+      </c>
+      <c r="B79" s="26"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="26"/>
+      <c r="E79" s="26"/>
+      <c r="F79" s="26"/>
+      <c r="G79" s="26"/>
+      <c r="H79" s="26"/>
+      <c r="I79" s="26"/>
+      <c r="J79" s="26"/>
+      <c r="K79" s="26"/>
+      <c r="L79" s="27"/>
+      <c r="M79" s="48"/>
+    </row>
+    <row r="80" spans="1:16" ht="20" x14ac:dyDescent="0.25">
+      <c r="A80" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="B80" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="C80" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="D80" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="E80" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F80" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="G80" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="H80" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="I80" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="J80" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="K80" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L80" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M80" s="48"/>
+    </row>
+    <row r="81" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <v>250</v>
+      </c>
+      <c r="B81" s="4">
+        <v>28</v>
+      </c>
+      <c r="C81" s="4">
+        <v>31</v>
+      </c>
+      <c r="D81" s="5">
+        <v>34</v>
+      </c>
+      <c r="E81" s="20">
+        <v>250</v>
+      </c>
+      <c r="F81" s="4">
+        <v>37</v>
+      </c>
+      <c r="G81" s="4">
+        <v>40</v>
+      </c>
+      <c r="H81" s="5">
+        <v>43</v>
+      </c>
+      <c r="I81" s="20">
+        <v>250</v>
+      </c>
+      <c r="J81" s="4">
+        <v>46</v>
+      </c>
+      <c r="K81" s="4">
+        <v>49</v>
+      </c>
+      <c r="L81" s="5">
+        <v>52</v>
+      </c>
+      <c r="M81" s="48"/>
+    </row>
+    <row r="82" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A82" s="20">
+        <v>500</v>
+      </c>
+      <c r="B82" s="4">
+        <v>29</v>
+      </c>
+      <c r="C82" s="4">
+        <v>32</v>
+      </c>
+      <c r="D82" s="5">
+        <v>35</v>
+      </c>
+      <c r="E82" s="20">
+        <v>500</v>
+      </c>
+      <c r="F82" s="4">
+        <v>38</v>
+      </c>
+      <c r="G82" s="4">
+        <v>41</v>
+      </c>
+      <c r="H82" s="5">
+        <v>44</v>
+      </c>
+      <c r="I82" s="20">
+        <v>500</v>
+      </c>
+      <c r="J82" s="4">
+        <v>47</v>
+      </c>
+      <c r="K82" s="4">
+        <v>50</v>
+      </c>
+      <c r="L82" s="5">
+        <v>53</v>
+      </c>
+      <c r="M82" s="48"/>
+    </row>
+    <row r="83" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A83" s="20">
+        <v>1000</v>
+      </c>
+      <c r="B83" s="6">
+        <v>30</v>
+      </c>
+      <c r="C83" s="6">
+        <v>33</v>
+      </c>
+      <c r="D83" s="7">
+        <v>36</v>
+      </c>
+      <c r="E83" s="20">
+        <v>1000</v>
+      </c>
+      <c r="F83" s="6">
+        <v>39</v>
+      </c>
+      <c r="G83" s="6">
+        <v>42</v>
+      </c>
+      <c r="H83" s="7">
+        <v>45</v>
+      </c>
+      <c r="I83" s="20">
+        <v>1000</v>
+      </c>
+      <c r="J83" s="6">
+        <v>48</v>
+      </c>
+      <c r="K83" s="6">
+        <v>51</v>
+      </c>
+      <c r="L83" s="7">
+        <v>54</v>
+      </c>
+      <c r="M83" s="48"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A84" s="48"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="48"/>
+      <c r="D84" s="48"/>
+      <c r="E84" s="48"/>
+      <c r="F84" s="48"/>
+      <c r="G84" s="48"/>
+      <c r="H84" s="48"/>
+      <c r="I84" s="48"/>
+      <c r="J84" s="48"/>
+      <c r="K84" s="48"/>
+      <c r="L84" s="48"/>
+      <c r="M84" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A45:L45"/>
+    <mergeCell ref="A51:L51"/>
+    <mergeCell ref="A59:L59"/>
+    <mergeCell ref="A65:L65"/>
+    <mergeCell ref="A73:L73"/>
+    <mergeCell ref="A79:L79"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="A36:L36"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>